<commit_message>
Added articles for the first version
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Datum</t>
   </si>
@@ -55,6 +55,27 @@
   </si>
   <si>
     <t>22.20</t>
+  </si>
+  <si>
+    <t>zinecker</t>
+  </si>
+  <si>
+    <t>zinecker - 3 tables WTF</t>
+  </si>
+  <si>
+    <t>zinecker - tab 4-10</t>
+  </si>
+  <si>
+    <t>zinecker - zbytek tab</t>
+  </si>
+  <si>
+    <t>zinecker -text</t>
+  </si>
+  <si>
+    <t>zinecker - text - kurziva…</t>
+  </si>
+  <si>
+    <t>úpravy celkově</t>
   </si>
 </sst>
 </file>
@@ -434,7 +455,7 @@
   <dimension ref="A1:Q49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -686,9 +707,7 @@
       <c r="E11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="3">
-        <v>3.8194444444444441E-2</v>
-      </c>
+      <c r="F11" s="3"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="9"/>
@@ -726,10 +745,22 @@
       <c r="Q12" s="8"/>
     </row>
     <row r="13" spans="2:17">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="B13" s="2">
+        <v>41902</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" ref="F13" si="1">D13-C13</f>
+        <v>3.819444444444442E-2</v>
+      </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="9"/>
@@ -743,9 +774,19 @@
     </row>
     <row r="14" spans="2:17">
       <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="C14" s="3">
+        <v>0.78819444444444453</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" ref="F14" si="2">D14-C14</f>
+        <v>4.513888888888884E-2</v>
+      </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="9"/>
@@ -759,8 +800,15 @@
     </row>
     <row r="15" spans="2:17">
       <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="C15" s="3">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3.125E-2</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -775,9 +823,19 @@
     </row>
     <row r="16" spans="2:17">
       <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="C16" s="3">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" ref="F16:F19" si="3">D16-C16</f>
+        <v>7.6388888888888951E-2</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="9"/>
@@ -791,9 +849,19 @@
     </row>
     <row r="17" spans="2:17">
       <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="C17" s="3">
+        <v>0.78125</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="3"/>
+        <v>2.777777777777779E-2</v>
+      </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -807,8 +875,13 @@
     </row>
     <row r="18" spans="2:17">
       <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3">
+        <v>0.94097222222222221</v>
+      </c>
       <c r="D18" s="3"/>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
@@ -822,10 +895,22 @@
       <c r="Q18" s="8"/>
     </row>
     <row r="19" spans="2:17">
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="B19" s="2">
+        <v>41904</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.90625</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.96875</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="3"/>
+        <v>6.25E-2</v>
+      </c>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="9"/>

</xml_diff>